<commit_message>
added new files and mofiled an existing
</commit_message>
<xml_diff>
--- a/Resources/DataDriven_TestData.xlsx
+++ b/Resources/DataDriven_TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Firstname</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Test@127</t>
+  </si>
+  <si>
+    <t>Vandana06</t>
+  </si>
+  <si>
+    <t>NAir06</t>
+  </si>
+  <si>
+    <t>Test@128</t>
   </si>
 </sst>
 </file>
@@ -454,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +562,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7829844600</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -560,8 +583,9 @@
     <hyperlink ref="D4" r:id="rId3" display="Test@123"/>
     <hyperlink ref="D5" r:id="rId4" display="Test@123"/>
     <hyperlink ref="D6" r:id="rId5" display="Test@123"/>
+    <hyperlink ref="D7" r:id="rId6" display="Test@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>